<commit_message>
change interaction with site
</commit_message>
<xml_diff>
--- a/Data/Result/050522-060522.xlsx
+++ b/Data/Result/050522-060522.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\UiPath\Task 1\Data\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8697DA50-988B-4BB1-AEF1-131F6362D3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4728" yWindow="2448" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4728" yWindow="2448" windowWidth="17280" windowHeight="8964" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="June" sheetId="2" r:id="rId1"/>
     <sheet name="May" sheetId="5" r:id="rId2"/>
+    <sheet name="March" sheetId="6" r:id="rId3"/>
+    <sheet name="February" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+    <x:ext xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
@@ -26,13 +27,13 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
+    </x:ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="126">
   <si>
     <t>Дата</t>
   </si>
@@ -290,12 +291,132 @@
   </si>
   <si>
     <t>131.97820324005892</t>
+  </si>
+  <si>
+    <t>04.03.2024</t>
+  </si>
+  <si>
+    <t>0.60894</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>01.03.2024</t>
+  </si>
+  <si>
+    <t>0.60727</t>
+  </si>
+  <si>
+    <t>29.02.2024</t>
+  </si>
+  <si>
+    <t>0.6032</t>
+  </si>
+  <si>
+    <t>28.02.2024</t>
+  </si>
+  <si>
+    <t>0.61063</t>
+  </si>
+  <si>
+    <t>27.02.2024</t>
+  </si>
+  <si>
+    <t>0.61138</t>
+  </si>
+  <si>
+    <t>26.02.2024</t>
+  </si>
+  <si>
+    <t>0.61627</t>
+  </si>
+  <si>
+    <t>22.02.2024</t>
+  </si>
+  <si>
+    <t>0.61666</t>
+  </si>
+  <si>
+    <t>21.02.2024</t>
+  </si>
+  <si>
+    <t>0.61605</t>
+  </si>
+  <si>
+    <t>20.02.2024</t>
+  </si>
+  <si>
+    <t>0.61435</t>
+  </si>
+  <si>
+    <t>19.02.2024</t>
+  </si>
+  <si>
+    <t>0.61615</t>
+  </si>
+  <si>
+    <t>16.02.2024</t>
+  </si>
+  <si>
+    <t>0.61638</t>
+  </si>
+  <si>
+    <t>15.02.2024</t>
+  </si>
+  <si>
+    <t>0.61069</t>
+  </si>
+  <si>
+    <t>14.02.2024</t>
+  </si>
+  <si>
+    <t>0.607</t>
+  </si>
+  <si>
+    <t>13.02.2024</t>
+  </si>
+  <si>
+    <t>0.61068</t>
+  </si>
+  <si>
+    <t>12.02.2024</t>
+  </si>
+  <si>
+    <t>0.60961</t>
+  </si>
+  <si>
+    <t>09.02.2024</t>
+  </si>
+  <si>
+    <t>0.60837</t>
+  </si>
+  <si>
+    <t>08.02.2024</t>
+  </si>
+  <si>
+    <t>0.61651</t>
+  </si>
+  <si>
+    <t>07.02.2024</t>
+  </si>
+  <si>
+    <t>06.02.2024</t>
+  </si>
+  <si>
+    <t>0.61009</t>
+  </si>
+  <si>
+    <t>05.02.2024</t>
+  </si>
+  <si>
+    <t>0.61348</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -627,7 +748,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -741,10 +862,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -1178,4 +1299,554 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
 </file>
</xml_diff>